<commit_message>
single application opened - Yes No closed option - Change alert to textPane
</commit_message>
<xml_diff>
--- a/form.excel/So1CuaDemo.xlsx
+++ b/form.excel/So1CuaDemo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="37">
   <si>
     <t xml:space="preserve">Mã số chứng từ </t>
   </si>
@@ -103,6 +103,33 @@
   </si>
   <si>
     <t>quoc123</t>
+  </si>
+  <si>
+    <t>ưe</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>qưeqwe</t>
+  </si>
+  <si>
+    <t>ưeqqưe</t>
+  </si>
+  <si>
+    <t>áda123</t>
+  </si>
+  <si>
+    <t>qưe</t>
+  </si>
+  <si>
+    <t>qyiuc1</t>
+  </si>
+  <si>
+    <t>qưee</t>
+  </si>
+  <si>
+    <t>wr</t>
   </si>
 </sst>
 </file>
@@ -589,7 +616,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -734,6 +761,126 @@
         <v>1234.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1234.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="n">
+        <v>124.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12450.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="n">
+        <v>12450.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12450.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12390.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>

</xml_diff>